<commit_message>
Update microstates files to v1.3.2. Resonance structures and most geometric isomers eliminated.
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM01_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM01_microstate_IDs_with_2D_depiction.xlsx
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t>SM01_microstate_IDs_with_2D_depiction.csv</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Microstate List</t>
   </si>
   <si>
     <t>Molecule</t>
@@ -40,12 +40,6 @@
     <t>c1cc2c(cc1[O-])c3c(o2)C(=NCCC3)[O-]</t>
   </si>
   <si>
-    <t>SM01_micro003</t>
-  </si>
-  <si>
-    <t>c1cc2=[O+]C3=C(NCCCC3=c2cc1O)[O-]</t>
-  </si>
-  <si>
     <t>SM01_micro004</t>
   </si>
   <si>
@@ -62,12 +56,6 @@
   </si>
   <si>
     <t>c1cc2c(cc1[O-])c3c(o2)C(=[OH+])NCCC3</t>
-  </si>
-  <si>
-    <t>SM01_micro007</t>
-  </si>
-  <si>
-    <t>c1cc2=[O+]C3=C(NCCCC3=c2cc1[O-])[O-]</t>
   </si>
   <si>
     <t>SM01_micro008</t>
@@ -486,82 +474,6 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="22583775"/>
-          <a:ext cx="3175163" cy="3175163"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3175163</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>3338</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="tmp10.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="25755600"/>
-          <a:ext cx="3175163" cy="3175163"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3175163</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>3338</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="tmp11.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="28927425"/>
           <a:ext cx="3175163" cy="3175163"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -859,7 +771,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -950,22 +862,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Add microstate list files with canonical SMILES.
</commit_message>
<xml_diff>
--- a/physical_properties/pKa/microstates/SM01_microstate_IDs_with_2D_depiction.xlsx
+++ b/physical_properties/pKa/microstates/SM01_microstate_IDs_with_2D_depiction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Microstate List</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>canonical isomeric SMILES</t>
+  </si>
+  <si>
+    <t>canonical SMILES</t>
   </si>
   <si>
     <t>SM01_micro001</t>
@@ -780,14 +783,15 @@
     <col min="1" max="1" width="50.7109375" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1">
+    <row r="2" spans="1:4" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -797,69 +801,96 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="250.0" customHeight="1">
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="250.0" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1" ht="250.0" customHeight="1">
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="250.0" customHeight="1">
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>